<commit_message>
Update 28 May: add new uploads
</commit_message>
<xml_diff>
--- a/uploads/track/h7kk0lsao.xlsx
+++ b/uploads/track/h7kk0lsao.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
   <si>
     <t>mobile</t>
   </si>
@@ -68,6 +68,27 @@
   </si>
   <si>
     <t xml:space="preserve">તારીખ -૨૫-૦૪-૨૦૨૫ વાર - શુક્રવાર </t>
+  </si>
+  <si>
+    <t>ભનુભાઈ જીવરાજભાઈ સોજીત્રા</t>
+  </si>
+  <si>
+    <t>28/05/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">સ્વ. ભનુભાઇ જીવરાજભાઈ સોજિત્રા </t>
+  </si>
+  <si>
+    <t xml:space="preserve">તા.૨૮-૦૫–૨૦૨૫ વાર બુધવાર </t>
+  </si>
+  <si>
+    <t>9429558756</t>
+  </si>
+  <si>
+    <t>સ્વ. ભનુભાઈ જીવરાજભાઈ સોજીત્રા|</t>
+  </si>
+  <si>
+    <t>28/05/2025 | મંગળવાર</t>
   </si>
 </sst>
 </file>
@@ -444,7 +465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -532,6 +553,74 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>

<commit_message>
Update 06 Jully : add new uploads
</commit_message>
<xml_diff>
--- a/uploads/track/h7kk0lsao.xlsx
+++ b/uploads/track/h7kk0lsao.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
   <si>
     <t>mobile</t>
   </si>
@@ -89,6 +89,18 @@
   </si>
   <si>
     <t>28/05/2025 | મંગળવાર</t>
+  </si>
+  <si>
+    <t xml:space="preserve">સ્વ. બાબુભાઇ લખમણભાઇ કણક </t>
+  </si>
+  <si>
+    <t xml:space="preserve">તારીખ - ૦૬-૦૬-૨૦૨૫  વાર શુક્રવાર </t>
+  </si>
+  <si>
+    <t xml:space="preserve">સ્વ. કંચનબેન ધીરુભાઈ પાથર </t>
+  </si>
+  <si>
+    <t xml:space="preserve">તારીખ -૨૯-૦૬-૨૦૨૫ વાર - રવિવાર </t>
   </si>
 </sst>
 </file>
@@ -465,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -621,6 +633,40 @@
         <v>9</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>